<commit_message>
updated paper suppl files
</commit_message>
<xml_diff>
--- a/paper_supplemental_files/Fig3_SourceData_Bacilli_AGG_Met_genomes_info.xlsx
+++ b/paper_supplemental_files/Fig3_SourceData_Bacilli_AGG_Met_genomes_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shulgina/Google Drive/genetic code paper/supplement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96A9391-1025-B241-B66A-9187B4CD9089}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85953C98-812C-1546-A127-F19E5485309B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="460" windowWidth="48960" windowHeight="31540" xr2:uid="{43D3B795-32D0-1D4C-A93F-C3CF537C0D08}"/>
   </bookViews>
@@ -711,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A9A72D-EA13-8843-AE70-1604CB32D78C}">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="132" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>